<commit_message>
Search test cases Adding
</commit_message>
<xml_diff>
--- a/src/main/java/com/makemytrip/qa/testdata/MakeMyTrip_TestData.xlsx
+++ b/src/main/java/com/makemytrip/qa/testdata/MakeMyTrip_TestData.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="19965" windowHeight="5055" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Page" sheetId="1" r:id="rId1"/>
     <sheet name="Registration_Page" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1:R15"/>
 </workbook>
 </file>
 
@@ -415,7 +415,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -461,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -532,16 +532,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Data driven testing for flights booking
</commit_message>
<xml_diff>
--- a/src/main/java/com/makemytrip/qa/testdata/MakeMyTrip_TestData.xlsx
+++ b/src/main/java/com/makemytrip/qa/testdata/MakeMyTrip_TestData.xlsx
@@ -88,13 +88,13 @@
     <t>Monica</t>
   </si>
   <si>
-    <t>Anantha Reddy</t>
-  </si>
-  <si>
     <t>monica@yahoo.com</t>
   </si>
   <si>
     <t>Mumbai</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -627,7 +627,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -662,13 +662,13 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="7">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>16</v>
@@ -705,7 +705,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="5">
         <v>31</v>
@@ -714,10 +714,10 @@
         <v>22</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>